<commit_message>
revert merge devBranch into Req_Victoria
</commit_message>
<xml_diff>
--- a/E_Pause_EasyMode.xlsx
+++ b/E_Pause_EasyMode.xlsx
@@ -1,27 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliawilkinson/Documents/Fall 2019/Eclipse Workspace/WaveGame2019/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEBEC12-7C10-4D4D-9C2A-403C64B37A01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Stories" sheetId="1" r:id="rId1"/>
-    <sheet name="Test E01" sheetId="2" r:id="rId2"/>
+    <sheet state="visible" name="Stories" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Test E01" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -120,53 +111,41 @@
   </si>
   <si>
     <t>TC, VG</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <fonts count="7">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
+    <font/>
     <font>
       <b/>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -175,7 +154,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -185,85 +164,62 @@
     </fill>
   </fills>
   <borders count="8">
+    <border/>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -273,96 +229,107 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="29">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -552,24 +519,21 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +542,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -589,7 +553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -600,7 +564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4">
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
@@ -609,267 +573,182 @@
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" gridLines="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="5.5" customWidth="1"/>
+    <col customWidth="1" min="2" max="2" width="26.29"/>
+    <col customWidth="1" min="3" max="3" width="42.0"/>
+    <col customWidth="1" min="4" max="4" width="5.57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1">
+    <row r="1">
       <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A6" s="10" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B6" s="19"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+    </row>
+    <row r="7">
       <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A9" s="13">
-        <v>1</v>
-      </c>
-      <c r="B9" s="14" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A10" s="13">
-        <v>2</v>
-      </c>
-      <c r="B10" s="15" t="s">
+      <c r="D9" s="26"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="23">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A11" s="13">
-        <v>3</v>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="D10" s="26"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="23">
+        <v>3.0</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A12" s="13">
-        <v>4</v>
-      </c>
-      <c r="B12" s="15" t="s">
+      <c r="D11" s="26"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="23">
+        <v>4.0</v>
+      </c>
+      <c r="B12" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A13" s="8" t="s">
+      <c r="D12" s="26"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>